<commit_message>
Fixed SPI port spreadsheet and other doc cleanup
A mistake in the pinout diagram was corrected in commit bf2bec864f299681884a0b370ce6527de034c568 however the SPI port spreadsheet did not reflect the change.

spreadsheet updates:
- SCK for SPI(2) was Port2B, now corrected to Port2C
- fixed broken link to D-series pinouts.jpg

other updates:
- added labeled diagram to overview page
- fixed some typos
</commit_message>
<xml_diff>
--- a/doc_src/source/spi_ports.xlsx
+++ b/doc_src/source/spi_ports.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lustiga/Dropbox (HHMI)/Code/karpova_lab/pyControl/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lustiga/Dropbox (HHMI)/Code/karpova_lab/pyControl/Hardware Modules/DSeries_breakout/doc_src/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F8F0FA-50AA-544E-B668-7FA7DB102855}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309D848F-454A-C044-A201-0794C3D4879D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="3860" windowWidth="28040" windowHeight="17440" xr2:uid="{0478C823-48AE-F041-8950-CBC4F5956F0A}"/>
   </bookViews>
@@ -156,10 +156,10 @@
     <t>d-series Breakout port</t>
   </si>
   <si>
-    <t>https://karpova-lab.github.io/pyControl-D-Series-Breakout/_static/pinouts.png</t>
-  </si>
-  <si>
     <t>port function</t>
+  </si>
+  <si>
+    <t>https://karpova-lab.github.io/pyControl-D-Series-Breakout/_static/pinouts.jpg</t>
   </si>
 </sst>
 </file>
@@ -557,7 +557,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G10"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -585,7 +585,7 @@
         <v>39</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -724,7 +724,7 @@
         <v>2</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -781,7 +781,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>